<commit_message>
ADD, ENH: latest CSTQ version.
</commit_message>
<xml_diff>
--- a/Code_Segmentation/Matlab/Parameters.xlsx
+++ b/Code_Segmentation/Matlab/Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sokratis/Documents/MATLAB/CSTQ/Training/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/415702851f959aa9/Documents/GitHub/Cell_Segm_Track_Quant_MIVIC/Code_Segmentation/Matlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEE4CCC-D353-914C-BAFC-CDE2FB748626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{33C91559-4927-C14F-B677-CC7421DA6D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{765B30F0-495C-4143-BE6E-4DB7250C3C2A}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="500" windowWidth="27900" windowHeight="15300" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="37">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -497,6 +497,19 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -732,7 +745,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="19" applyFont="1"/>
@@ -787,9 +800,6 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -806,12 +816,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -848,13 +852,19 @@
     <xf numFmtId="0" fontId="23" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="79">
     <cellStyle name="Good" xfId="39" builtinId="26"/>
@@ -1216,35 +1226,35 @@
   <dimension ref="A1:AS74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B9" sqref="B9:U9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="9.1640625" style="1"/>
-    <col min="5" max="5" width="10.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="1" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="10.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" style="1" customWidth="1"/>
     <col min="19" max="19" width="16" style="1" customWidth="1"/>
     <col min="20" max="20" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="1037" width="8.5" style="1"/>
-    <col min="1038" max="16384" width="9.1640625" style="1"/>
+    <col min="21" max="21" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="1037" width="8.42578125" style="1"/>
+    <col min="1038" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="16">
+    <row r="1" spans="1:45" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1269,7 +1279,7 @@
       <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="44" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="29" t="s">
@@ -2143,7 +2153,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:45" ht="16">
+    <row r="8" spans="1:45" ht="15.75">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -2274,68 +2284,68 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:45" ht="16">
+    <row r="9" spans="1:45" ht="15.75">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="34">
-        <v>1</v>
-      </c>
-      <c r="C9" s="35">
-        <v>2</v>
-      </c>
-      <c r="D9" s="35">
-        <v>4</v>
-      </c>
-      <c r="E9" s="35">
-        <v>2.3E-2</v>
-      </c>
-      <c r="F9" s="35">
-        <v>2</v>
-      </c>
-      <c r="G9" s="35">
-        <v>0.1</v>
-      </c>
-      <c r="H9" s="35">
-        <v>10</v>
-      </c>
-      <c r="I9" s="35">
+      <c r="B9" s="58">
+        <v>1</v>
+      </c>
+      <c r="C9" s="58">
+        <v>2</v>
+      </c>
+      <c r="D9" s="58">
+        <v>4</v>
+      </c>
+      <c r="E9" s="58">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F9" s="58">
+        <v>2</v>
+      </c>
+      <c r="G9" s="58">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="58">
+        <v>15</v>
+      </c>
+      <c r="I9" s="58">
         <v>60</v>
       </c>
-      <c r="J9" s="35">
-        <v>4</v>
-      </c>
-      <c r="K9" s="35">
-        <v>3</v>
-      </c>
-      <c r="L9" s="35">
-        <v>6</v>
-      </c>
-      <c r="M9" s="35">
-        <v>4</v>
-      </c>
-      <c r="N9" s="35">
+      <c r="J9" s="58">
+        <v>4</v>
+      </c>
+      <c r="K9" s="58">
+        <v>3</v>
+      </c>
+      <c r="L9" s="58">
+        <v>4</v>
+      </c>
+      <c r="M9" s="58">
+        <v>8</v>
+      </c>
+      <c r="N9" s="58">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="O9" s="35">
-        <v>2</v>
-      </c>
-      <c r="P9" s="35">
-        <v>10</v>
-      </c>
-      <c r="Q9" s="35">
-        <v>1</v>
-      </c>
-      <c r="R9" s="35">
+      <c r="O9" s="58">
+        <v>2</v>
+      </c>
+      <c r="P9" s="58">
+        <v>30</v>
+      </c>
+      <c r="Q9" s="58">
+        <v>1</v>
+      </c>
+      <c r="R9" s="58">
         <v>14</v>
       </c>
-      <c r="S9" s="35">
+      <c r="S9" s="58">
         <v>9</v>
       </c>
-      <c r="T9" s="35">
-        <v>5</v>
-      </c>
-      <c r="U9" s="35">
+      <c r="T9" s="58">
+        <v>5</v>
+      </c>
+      <c r="U9" s="58">
         <v>0.5</v>
       </c>
       <c r="V9" s="7"/>
@@ -2409,64 +2419,64 @@
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="50">
-        <v>1</v>
-      </c>
-      <c r="C10" s="51">
-        <v>1</v>
-      </c>
-      <c r="D10" s="51">
+      <c r="B10" s="47">
+        <v>1</v>
+      </c>
+      <c r="C10" s="48">
+        <v>1</v>
+      </c>
+      <c r="D10" s="48">
         <v>14</v>
       </c>
-      <c r="E10" s="51">
+      <c r="E10" s="48">
         <v>0.04</v>
       </c>
-      <c r="F10" s="51">
-        <v>2</v>
-      </c>
-      <c r="G10" s="51">
-        <v>0.1</v>
-      </c>
-      <c r="H10" s="51">
+      <c r="F10" s="48">
+        <v>2</v>
+      </c>
+      <c r="G10" s="48">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="48">
         <v>60</v>
       </c>
-      <c r="I10" s="51">
+      <c r="I10" s="48">
         <v>30</v>
       </c>
-      <c r="J10" s="51">
-        <v>3</v>
-      </c>
-      <c r="K10" s="51">
-        <v>3</v>
-      </c>
-      <c r="L10" s="51">
-        <v>3</v>
-      </c>
-      <c r="M10" s="51">
+      <c r="J10" s="48">
+        <v>3</v>
+      </c>
+      <c r="K10" s="48">
+        <v>3</v>
+      </c>
+      <c r="L10" s="48">
+        <v>3</v>
+      </c>
+      <c r="M10" s="48">
         <v>1.5</v>
       </c>
-      <c r="N10" s="52">
+      <c r="N10" s="49">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O10" s="51">
-        <v>2</v>
-      </c>
-      <c r="P10" s="51">
+      <c r="O10" s="48">
+        <v>2</v>
+      </c>
+      <c r="P10" s="48">
         <v>50</v>
       </c>
-      <c r="Q10" s="51">
-        <v>0.5</v>
-      </c>
-      <c r="R10" s="51">
+      <c r="Q10" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="R10" s="48">
         <v>0.3</v>
       </c>
-      <c r="S10" s="51">
+      <c r="S10" s="48">
         <v>9</v>
       </c>
-      <c r="T10" s="51">
-        <v>5</v>
-      </c>
-      <c r="U10" s="51">
+      <c r="T10" s="48">
+        <v>5</v>
+      </c>
+      <c r="U10" s="48">
         <v>0.5</v>
       </c>
       <c r="V10" s="5"/>
@@ -2536,68 +2546,68 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:45" ht="16">
+    <row r="11" spans="1:45" ht="15.75">
       <c r="A11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="36">
-        <v>1</v>
-      </c>
-      <c r="C11" s="37">
-        <v>1</v>
-      </c>
-      <c r="D11" s="37">
+      <c r="B11" s="35">
+        <v>1</v>
+      </c>
+      <c r="C11" s="36">
+        <v>1</v>
+      </c>
+      <c r="D11" s="36">
         <v>22</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11" s="36">
         <v>5.7516627813386498E-2</v>
       </c>
-      <c r="F11" s="37">
-        <v>2</v>
-      </c>
-      <c r="G11" s="37">
-        <v>0.1</v>
-      </c>
-      <c r="H11" s="37">
-        <v>3</v>
-      </c>
-      <c r="I11" s="37">
+      <c r="F11" s="36">
+        <v>2</v>
+      </c>
+      <c r="G11" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="36">
+        <v>3</v>
+      </c>
+      <c r="I11" s="36">
         <v>60</v>
       </c>
-      <c r="J11" s="37">
-        <v>3</v>
-      </c>
-      <c r="K11" s="37">
-        <v>3</v>
-      </c>
-      <c r="L11" s="37">
-        <v>3</v>
-      </c>
-      <c r="M11" s="37">
-        <v>2</v>
-      </c>
-      <c r="N11" s="37">
+      <c r="J11" s="36">
+        <v>3</v>
+      </c>
+      <c r="K11" s="36">
+        <v>3</v>
+      </c>
+      <c r="L11" s="36">
+        <v>3</v>
+      </c>
+      <c r="M11" s="36">
+        <v>2</v>
+      </c>
+      <c r="N11" s="36">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O11" s="37">
-        <v>2</v>
-      </c>
-      <c r="P11" s="37">
-        <v>5</v>
-      </c>
-      <c r="Q11" s="37">
+      <c r="O11" s="36">
+        <v>2</v>
+      </c>
+      <c r="P11" s="36">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="36">
         <v>0.01</v>
       </c>
-      <c r="R11" s="37">
+      <c r="R11" s="36">
         <v>0.25</v>
       </c>
-      <c r="S11" s="37">
+      <c r="S11" s="36">
         <v>9</v>
       </c>
-      <c r="T11" s="35">
-        <v>5</v>
-      </c>
-      <c r="U11" s="37">
+      <c r="T11" s="34">
+        <v>5</v>
+      </c>
+      <c r="U11" s="36">
         <v>0.5</v>
       </c>
       <c r="V11" s="5"/>
@@ -2667,68 +2677,68 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:45" ht="16">
+    <row r="12" spans="1:45" ht="15.75">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="38">
-        <v>1</v>
-      </c>
-      <c r="C12" s="39">
-        <v>1</v>
-      </c>
-      <c r="D12" s="39">
+      <c r="B12" s="37">
+        <v>1</v>
+      </c>
+      <c r="C12" s="38">
+        <v>1</v>
+      </c>
+      <c r="D12" s="38">
         <v>18</v>
       </c>
-      <c r="E12" s="39">
+      <c r="E12" s="38">
         <v>0.05</v>
       </c>
-      <c r="F12" s="39">
-        <v>2</v>
-      </c>
-      <c r="G12" s="39">
-        <v>0.1</v>
-      </c>
-      <c r="H12" s="39">
+      <c r="F12" s="38">
+        <v>2</v>
+      </c>
+      <c r="G12" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="38">
         <v>110</v>
       </c>
-      <c r="I12" s="39">
+      <c r="I12" s="38">
         <v>60</v>
       </c>
-      <c r="J12" s="39">
+      <c r="J12" s="38">
         <v>3.5</v>
       </c>
-      <c r="K12" s="39">
-        <v>3</v>
-      </c>
-      <c r="L12" s="39">
+      <c r="K12" s="38">
+        <v>3</v>
+      </c>
+      <c r="L12" s="38">
         <v>3.5</v>
       </c>
-      <c r="M12" s="39">
-        <v>2</v>
-      </c>
-      <c r="N12" s="40">
+      <c r="M12" s="38">
+        <v>2</v>
+      </c>
+      <c r="N12" s="39">
         <v>0.01</v>
       </c>
-      <c r="O12" s="39">
-        <v>2</v>
-      </c>
-      <c r="P12" s="39">
+      <c r="O12" s="38">
+        <v>2</v>
+      </c>
+      <c r="P12" s="38">
         <v>0</v>
       </c>
-      <c r="Q12" s="39">
-        <v>1</v>
-      </c>
-      <c r="R12" s="39">
-        <v>2</v>
-      </c>
-      <c r="S12" s="39">
+      <c r="Q12" s="38">
+        <v>1</v>
+      </c>
+      <c r="R12" s="38">
+        <v>2</v>
+      </c>
+      <c r="S12" s="38">
         <v>9</v>
       </c>
-      <c r="T12" s="39">
-        <v>5</v>
-      </c>
-      <c r="U12" s="39">
+      <c r="T12" s="38">
+        <v>5</v>
+      </c>
+      <c r="U12" s="38">
         <v>0.5</v>
       </c>
       <c r="V12" s="7"/>
@@ -2798,68 +2808,68 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:45" ht="16">
+    <row r="13" spans="1:45" ht="15.75">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="41">
-        <v>1</v>
-      </c>
-      <c r="C13" s="42">
-        <v>1</v>
-      </c>
-      <c r="D13" s="42">
-        <v>8</v>
-      </c>
-      <c r="E13" s="42">
-        <v>0.05</v>
-      </c>
-      <c r="F13" s="42">
-        <v>2</v>
-      </c>
-      <c r="G13" s="41">
-        <v>0.1</v>
-      </c>
-      <c r="H13" s="41">
-        <v>24</v>
-      </c>
-      <c r="I13" s="41">
+      <c r="B13" s="53">
+        <v>1</v>
+      </c>
+      <c r="C13" s="54">
+        <v>1</v>
+      </c>
+      <c r="D13" s="54">
+        <v>14</v>
+      </c>
+      <c r="E13" s="54">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="F13" s="54">
+        <v>2</v>
+      </c>
+      <c r="G13" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="53">
+        <v>22</v>
+      </c>
+      <c r="I13" s="53">
         <v>60</v>
       </c>
-      <c r="J13" s="41">
-        <v>4</v>
-      </c>
-      <c r="K13" s="42">
-        <v>3</v>
-      </c>
-      <c r="L13" s="41">
-        <v>3</v>
-      </c>
-      <c r="M13" s="41">
-        <v>2</v>
-      </c>
-      <c r="N13" s="42">
+      <c r="J13" s="53">
+        <v>4</v>
+      </c>
+      <c r="K13" s="54">
+        <v>3</v>
+      </c>
+      <c r="L13" s="53">
+        <v>3</v>
+      </c>
+      <c r="M13" s="53">
+        <v>3</v>
+      </c>
+      <c r="N13" s="54">
         <v>0.01</v>
       </c>
-      <c r="O13" s="42">
-        <v>2</v>
-      </c>
-      <c r="P13" s="42">
-        <v>35</v>
-      </c>
-      <c r="Q13" s="41">
+      <c r="O13" s="54">
+        <v>2</v>
+      </c>
+      <c r="P13" s="54">
+        <v>45</v>
+      </c>
+      <c r="Q13" s="53">
         <v>1E-3</v>
       </c>
-      <c r="R13" s="41">
+      <c r="R13" s="53">
         <v>50</v>
       </c>
-      <c r="S13" s="41">
+      <c r="S13" s="53">
         <v>9</v>
       </c>
-      <c r="T13" s="35">
-        <v>5</v>
-      </c>
-      <c r="U13" s="42">
+      <c r="T13" s="55">
+        <v>5</v>
+      </c>
+      <c r="U13" s="54">
         <v>0.5</v>
       </c>
       <c r="V13" s="7"/>
@@ -2933,64 +2943,64 @@
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="43">
-        <v>1</v>
-      </c>
-      <c r="C14" s="44">
-        <v>1</v>
-      </c>
-      <c r="D14" s="44">
-        <v>8</v>
-      </c>
-      <c r="E14" s="44">
+      <c r="B14" s="40">
+        <v>1</v>
+      </c>
+      <c r="C14" s="41">
+        <v>1</v>
+      </c>
+      <c r="D14" s="41">
+        <v>8</v>
+      </c>
+      <c r="E14" s="41">
         <v>0.03</v>
       </c>
-      <c r="F14" s="44">
-        <v>2</v>
-      </c>
-      <c r="G14" s="45">
-        <v>0.1</v>
-      </c>
-      <c r="H14" s="45">
-        <v>5</v>
-      </c>
-      <c r="I14" s="45">
+      <c r="F14" s="41">
+        <v>2</v>
+      </c>
+      <c r="G14" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="H14" s="42">
+        <v>5</v>
+      </c>
+      <c r="I14" s="42">
         <v>60</v>
       </c>
-      <c r="J14" s="44">
+      <c r="J14" s="41">
         <v>2.5</v>
       </c>
-      <c r="K14" s="44">
-        <v>3</v>
-      </c>
-      <c r="L14" s="44">
+      <c r="K14" s="41">
+        <v>3</v>
+      </c>
+      <c r="L14" s="41">
         <v>2.5</v>
       </c>
-      <c r="M14" s="45">
-        <v>2</v>
-      </c>
-      <c r="N14" s="46">
+      <c r="M14" s="42">
+        <v>2</v>
+      </c>
+      <c r="N14" s="43">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="O14" s="44">
-        <v>2</v>
-      </c>
-      <c r="P14" s="45">
-        <v>5</v>
-      </c>
-      <c r="Q14" s="45">
-        <v>1</v>
-      </c>
-      <c r="R14" s="45">
-        <v>5</v>
-      </c>
-      <c r="S14" s="44">
+      <c r="O14" s="41">
+        <v>2</v>
+      </c>
+      <c r="P14" s="42">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="42">
+        <v>1</v>
+      </c>
+      <c r="R14" s="42">
+        <v>5</v>
+      </c>
+      <c r="S14" s="41">
         <v>9</v>
       </c>
-      <c r="T14" s="44">
-        <v>5</v>
-      </c>
-      <c r="U14" s="44">
+      <c r="T14" s="41">
+        <v>5</v>
+      </c>
+      <c r="U14" s="41">
         <v>0.5</v>
       </c>
       <c r="V14" s="7"/>
@@ -3060,68 +3070,68 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:45" ht="16">
+    <row r="15" spans="1:45" ht="15.75">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="48">
-        <v>1</v>
-      </c>
-      <c r="C15" s="48">
-        <v>1</v>
-      </c>
-      <c r="D15" s="48">
-        <v>8</v>
-      </c>
-      <c r="E15" s="57">
+      <c r="B15" s="45">
+        <v>1</v>
+      </c>
+      <c r="C15" s="45">
+        <v>1</v>
+      </c>
+      <c r="D15" s="45">
+        <v>8</v>
+      </c>
+      <c r="E15" s="52">
         <v>0.18437008724204099</v>
       </c>
-      <c r="F15" s="48">
-        <v>1</v>
-      </c>
-      <c r="G15" s="48">
-        <v>0.1</v>
-      </c>
-      <c r="H15" s="48">
-        <v>1</v>
-      </c>
-      <c r="I15" s="48">
+      <c r="F15" s="45">
+        <v>1</v>
+      </c>
+      <c r="G15" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="45">
+        <v>1</v>
+      </c>
+      <c r="I15" s="45">
         <v>75</v>
       </c>
-      <c r="J15" s="48">
-        <v>3</v>
-      </c>
-      <c r="K15" s="48">
-        <v>3</v>
-      </c>
-      <c r="L15" s="48">
+      <c r="J15" s="45">
+        <v>3</v>
+      </c>
+      <c r="K15" s="45">
+        <v>3</v>
+      </c>
+      <c r="L15" s="45">
         <v>40</v>
       </c>
-      <c r="M15" s="48">
-        <v>3</v>
-      </c>
-      <c r="N15" s="48">
+      <c r="M15" s="45">
+        <v>3</v>
+      </c>
+      <c r="N15" s="45">
         <v>1E-3</v>
       </c>
-      <c r="O15" s="48">
-        <v>2</v>
-      </c>
-      <c r="P15" s="48">
+      <c r="O15" s="45">
+        <v>2</v>
+      </c>
+      <c r="P15" s="45">
         <v>50</v>
       </c>
-      <c r="Q15" s="48">
+      <c r="Q15" s="45">
         <v>0.01</v>
       </c>
-      <c r="R15" s="48">
+      <c r="R15" s="45">
         <v>50</v>
       </c>
-      <c r="S15" s="48">
+      <c r="S15" s="45">
         <v>9</v>
       </c>
-      <c r="T15" s="49">
-        <v>5</v>
-      </c>
-      <c r="U15" s="48">
+      <c r="T15" s="46">
+        <v>5</v>
+      </c>
+      <c r="U15" s="45">
         <v>0.5</v>
       </c>
       <c r="V15" s="5"/>
@@ -3191,68 +3201,68 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:45" ht="16">
+    <row r="16" spans="1:45" ht="15.75">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="53">
-        <v>1</v>
-      </c>
-      <c r="C16" s="53">
-        <v>1</v>
-      </c>
-      <c r="D16" s="53">
+      <c r="B16" s="50">
+        <v>1</v>
+      </c>
+      <c r="C16" s="50">
+        <v>1</v>
+      </c>
+      <c r="D16" s="50">
         <v>12</v>
       </c>
-      <c r="E16" s="53">
+      <c r="E16" s="50">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="F16" s="53">
-        <v>2</v>
-      </c>
-      <c r="G16" s="54">
-        <v>0.1</v>
-      </c>
-      <c r="H16" s="54">
+      <c r="F16" s="50">
+        <v>2</v>
+      </c>
+      <c r="G16" s="51">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="51">
         <v>12</v>
       </c>
-      <c r="I16" s="54">
+      <c r="I16" s="51">
         <v>30</v>
       </c>
-      <c r="J16" s="54">
-        <v>4</v>
-      </c>
-      <c r="K16" s="53">
-        <v>3</v>
-      </c>
-      <c r="L16" s="54">
+      <c r="J16" s="51">
+        <v>4</v>
+      </c>
+      <c r="K16" s="50">
+        <v>3</v>
+      </c>
+      <c r="L16" s="51">
         <v>6</v>
       </c>
-      <c r="M16" s="54">
-        <v>4</v>
-      </c>
-      <c r="N16" s="53">
-        <v>0.1</v>
-      </c>
-      <c r="O16" s="54">
-        <v>1</v>
-      </c>
-      <c r="P16" s="54">
+      <c r="M16" s="51">
+        <v>4</v>
+      </c>
+      <c r="N16" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="O16" s="51">
+        <v>1</v>
+      </c>
+      <c r="P16" s="51">
         <v>10</v>
       </c>
-      <c r="Q16" s="54">
-        <v>4</v>
-      </c>
-      <c r="R16" s="54">
+      <c r="Q16" s="51">
+        <v>4</v>
+      </c>
+      <c r="R16" s="51">
         <v>100</v>
       </c>
-      <c r="S16" s="54">
+      <c r="S16" s="51">
         <v>10</v>
       </c>
-      <c r="T16" s="54">
-        <v>5</v>
-      </c>
-      <c r="U16" s="53">
+      <c r="T16" s="51">
+        <v>5</v>
+      </c>
+      <c r="U16" s="50">
         <v>0.5</v>
       </c>
       <c r="W16" s="6"/>
@@ -3321,68 +3331,68 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:45" ht="16">
+    <row r="17" spans="1:45" ht="15.75">
       <c r="A17" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="55">
-        <v>1</v>
-      </c>
-      <c r="C17" s="55">
-        <v>1</v>
-      </c>
-      <c r="D17" s="55">
+      <c r="B17" s="56">
+        <v>1</v>
+      </c>
+      <c r="C17" s="56">
+        <v>1</v>
+      </c>
+      <c r="D17" s="56">
         <v>12</v>
       </c>
-      <c r="E17" s="55">
+      <c r="E17" s="56">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F17" s="55">
-        <v>2</v>
-      </c>
-      <c r="G17" s="56">
-        <v>0.1</v>
-      </c>
-      <c r="H17" s="56">
-        <v>8</v>
-      </c>
-      <c r="I17" s="56">
+      <c r="F17" s="56">
+        <v>2</v>
+      </c>
+      <c r="G17" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="57">
+        <v>8</v>
+      </c>
+      <c r="I17" s="57">
         <v>20</v>
       </c>
-      <c r="J17" s="56">
-        <v>4</v>
-      </c>
-      <c r="K17" s="55">
-        <v>3</v>
-      </c>
-      <c r="L17" s="56">
+      <c r="J17" s="57">
+        <v>4</v>
+      </c>
+      <c r="K17" s="56">
+        <v>3</v>
+      </c>
+      <c r="L17" s="57">
         <v>6</v>
       </c>
-      <c r="M17" s="56">
-        <v>4</v>
-      </c>
-      <c r="N17" s="55">
-        <v>0.1</v>
-      </c>
-      <c r="O17" s="56">
-        <v>1</v>
-      </c>
-      <c r="P17" s="56">
-        <v>8</v>
-      </c>
-      <c r="Q17" s="56">
-        <v>4</v>
-      </c>
-      <c r="R17" s="56">
+      <c r="M17" s="57">
+        <v>4</v>
+      </c>
+      <c r="N17" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="O17" s="57">
+        <v>1</v>
+      </c>
+      <c r="P17" s="57">
+        <v>8</v>
+      </c>
+      <c r="Q17" s="57">
+        <v>4</v>
+      </c>
+      <c r="R17" s="57">
         <v>100</v>
       </c>
-      <c r="S17" s="56">
+      <c r="S17" s="57">
         <v>10</v>
       </c>
-      <c r="T17" s="56">
-        <v>5</v>
-      </c>
-      <c r="U17" s="55">
+      <c r="T17" s="57">
+        <v>5</v>
+      </c>
+      <c r="U17" s="56">
         <v>0.5</v>
       </c>
       <c r="V17" s="7"/>

</xml_diff>